<commit_message>
comparison does not work properly
</commit_message>
<xml_diff>
--- a/price.xlsx
+++ b/price.xlsx
@@ -817,12 +817,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -1206,11 +1205,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1234,7 +1233,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1270,7 +1269,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1298,7 +1297,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1342,11 +1341,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1358,7 +1357,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1402,11 +1401,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1517,10 +1516,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="1" sqref="C:C B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="1" max="5" min="3" style="0" width="12.63"/>
@@ -31685,10 +31684,10 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C229" activeCellId="0" sqref="C229"/>
+      <selection pane="topLeft" activeCell="C199" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="3" min="3" style="41" width="17.21"/>

</xml_diff>